<commit_message>
add comments for model3
</commit_message>
<xml_diff>
--- a/data/stock-forecaster-vix-sp500.xlsx
+++ b/data/stock-forecaster-vix-sp500.xlsx
@@ -19,10 +19,10 @@
     <t>date</t>
   </si>
   <si>
-    <t>^VIX_close</t>
+    <t>VIX_close</t>
   </si>
   <si>
-    <t>^GSPC_close</t>
+    <t>SP500_close</t>
   </si>
   <si>
     <t>future_result</t>

</xml_diff>